<commit_message>
update of statistic lecture
Signed-off-by: Yong-iL Joh <jsjjsmith888@gmail.com>
</commit_message>
<xml_diff>
--- a/R.2019.2/sample.survey/sample.survey.03.xlsx
+++ b/R.2019.2/sample.survey/sample.survey.03.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkien/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkien/work/misc/R.2019.2/sample.survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10C967D-A4EF-154C-838E-408B8CE38A1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185662A3-2690-1149-B4C9-2A055F01D62E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="16100" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="16100" windowHeight="14600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="homework" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>종로구</t>
   </si>
@@ -169,6 +169,70 @@
   </si>
   <si>
     <t>z_(a/2) ~= 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>n0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B (절대오차한계)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>n_est</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>n_0 / (1 + n_0 / N)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>숙제 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>숙제 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>p^</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(z_(a/2)*S)^2 / B^2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>((N-n)/N)*(p^*q^/(n-1))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(N-n)/N ~=</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>z_(a/2) ~=</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(z_(a/2)^2*p*q) / B^2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>z_(a/2) =~</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -176,11 +240,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="#,##0_ "/>
+    <numFmt numFmtId="178" formatCode="m&quot;월&quot;\ d&quot;일&quot;"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
@@ -263,6 +328,19 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -308,7 +386,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -365,6 +443,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="쉼표 [0] 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -708,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -1326,12 +1408,296 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="22">
+        <v>20000</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="22">
+        <v>300</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="25">
+        <v>431</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="22">
+        <v>320</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="22">
+        <f>((C$2-C$3)/C$2)*C$5/C$3</f>
+        <v>1.0506666666666666</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="22">
+        <f>SQRT(C7)</f>
+        <v>1.0250203250017371</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="22">
+        <f>C8*E10</f>
+        <v>2.0500406500034742</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="2:6" ht="17">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="22">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <f>_xlfn.NORM.INV(1-0.05/2, 0, 1)</f>
+        <v>1.9599639845400536</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="25">
+        <f>C4-C9</f>
+        <v>428.9499593499965</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="25">
+        <f>C4+C9</f>
+        <v>433.0500406500035</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="22">
+        <v>2</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="22">
+        <f>(E10 *SQRT(C5) )^2/C14^2</f>
+        <v>320.00000000000006</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="22">
+        <f>C15/(1+C15/C2)</f>
+        <v>314.96062992125991</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <f>870/C21</f>
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <f>E25*(C22*(1-C22))/(C21-1)</f>
+        <v>1.6250833889259507E-4</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="22"/>
+      <c r="D25" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="22">
+        <f>SQRT(C24)</f>
+        <v>1.2747875858063376E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="22">
+        <f>C26*E28</f>
+        <v>2.5495751716126752E-2</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="22"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="D28" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="22">
+        <v>0.03</v>
+      </c>
+      <c r="D30" s="22"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="22">
+        <f>(E28^2*C22*(1-C22))/C30^2</f>
+        <v>1082.6666666666667</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="24"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>